<commit_message>
Updated example protocol spreadsheet to new format
</commit_message>
<xml_diff>
--- a/Main/NEW_PROTOCOL/Protocol.xlsx
+++ b/Main/NEW_PROTOCOL/Protocol.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Protocol Name</t>
   </si>
@@ -23,13 +23,16 @@
     <t>Protocol Actions</t>
   </si>
   <si>
+    <t>Pack</t>
+  </si>
+  <si>
     <t>Creator Tag</t>
   </si>
   <si>
     <t>Homebrew</t>
   </si>
   <si>
-    <t>&gt;Let imagination grow.</t>
+    <t>Let imagination grow.</t>
   </si>
   <si>
     <t>Shift, Draw</t>
@@ -143,14 +146,14 @@
   <borders count="4">
     <border/>
     <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -164,29 +167,32 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -413,9 +419,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="17.13"/>
-    <col customWidth="1" min="2" max="2" width="64.63"/>
-    <col customWidth="1" min="3" max="3" width="83.88"/>
-    <col customWidth="1" min="4" max="4" width="48.13"/>
+    <col customWidth="1" min="2" max="2" width="19.75"/>
+    <col customWidth="1" min="3" max="3" width="15.0"/>
+    <col customWidth="1" min="4" max="5" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -431,19 +437,23 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -464,70 +474,71 @@
     <col customWidth="1" min="2" max="2" width="14.38"/>
     <col customWidth="1" min="3" max="3" width="6.38"/>
     <col customWidth="1" min="4" max="4" width="27.5"/>
-    <col customWidth="1" min="5" max="5" width="47.63"/>
+    <col customWidth="1" min="5" max="5" width="39.38"/>
     <col customWidth="1" min="6" max="6" width="18.38"/>
     <col customWidth="1" min="7" max="7" width="22.25"/>
-    <col customWidth="1" min="8" max="9" width="47.63"/>
+    <col customWidth="1" min="8" max="8" width="17.63"/>
+    <col customWidth="1" min="9" max="9" width="13.13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F1" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7">
         <v>0.0</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7">
         <v>1.0</v>
@@ -537,50 +548,50 @@
       <c r="F3" s="8"/>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="7">
         <v>2.0</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7">
         <v>3.0</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="7"/>
@@ -589,17 +600,17 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="7">
         <v>4.0</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="7"/>
@@ -608,10 +619,10 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="7">
         <v>5.0</v>
@@ -620,10 +631,10 @@
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>